<commit_message>
data sheet update to  4 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,6 +735,17 @@
       </c>
       <c r="C28" s="2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>43925</v>
+      </c>
+      <c r="B29" s="2">
+        <v>70</v>
+      </c>
+      <c r="C29" s="2">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -750,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,6 +1082,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>43925</v>
+      </c>
+      <c r="B29" s="2">
+        <v>30</v>
+      </c>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1080,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,6 +1423,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>43925</v>
+      </c>
+      <c r="B29" s="1">
+        <v>8</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Data Set 5 april 2020
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,6 +746,17 @@
       </c>
       <c r="C29" s="2">
         <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>43926</v>
+      </c>
+      <c r="B30" s="2">
+        <v>88</v>
+      </c>
+      <c r="C30" s="2">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -761,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,6 +1104,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>43926</v>
+      </c>
+      <c r="B30" s="2">
+        <v>30</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1102,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,6 +1456,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>43926</v>
+      </c>
+      <c r="B30" s="1">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update dataset to 6 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Death!$A$1:$C$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recoverd!$A$1:$C$28</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -416,9 +416,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -757,6 +757,18 @@
       </c>
       <c r="C30" s="2">
         <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>43927</v>
+      </c>
+      <c r="B31" s="2">
+        <f>SUM(B30+C31)</f>
+        <v>123</v>
+      </c>
+      <c r="C31" s="2">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -772,10 +784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,6 +1127,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>43927</v>
+      </c>
+      <c r="B31" s="2">
+        <f>SUM(B30+C31)</f>
+        <v>33</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1124,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,6 +1491,18 @@
         <v>1</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>43927</v>
+      </c>
+      <c r="B31" s="2">
+        <f>SUM(B30+C31)</f>
+        <v>12</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update some errors on data
recovered count was wrong .
corrected
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1061,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,10 +1135,10 @@
         <v>43924</v>
       </c>
       <c r="B28" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1149,7 +1149,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,10 +1157,10 @@
         <v>43926</v>
       </c>
       <c r="B30" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1168,11 +1168,10 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f>SUM(B30+C31)</f>
         <v>33</v>
       </c>
       <c r="C31" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1180,7 +1179,6 @@
         <v>43928</v>
       </c>
       <c r="B32" s="2">
-        <f>SUM(B31+C32)</f>
         <v>33</v>
       </c>
       <c r="C32" s="2">
@@ -1192,7 +1190,6 @@
         <v>43929</v>
       </c>
       <c r="B33" s="2">
-        <f>SUM(B32+C33)</f>
         <v>33</v>
       </c>
       <c r="C33" s="2">
@@ -1204,7 +1201,6 @@
         <v>43930</v>
       </c>
       <c r="B34" s="2">
-        <f>SUM(B33+C34)</f>
         <v>33</v>
       </c>
       <c r="C34" s="2">

</xml_diff>

<commit_message>
Dataset update 10 april
last update 10 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,6 +805,18 @@
       </c>
       <c r="C34" s="2">
         <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>43931</v>
+      </c>
+      <c r="B35" s="2">
+        <f>SUM(B34+C35)</f>
+        <v>424</v>
+      </c>
+      <c r="C35" s="2">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -820,10 +832,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,6 +1219,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>43931</v>
+      </c>
+      <c r="B35" s="2">
+        <v>33</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1216,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B34"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,6 +1630,18 @@
         <v>1</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>43931</v>
+      </c>
+      <c r="B35" s="2">
+        <f>SUM(B34+C35)</f>
+        <v>27</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data update 11 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,6 +817,18 @@
       </c>
       <c r="C35" s="2">
         <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>43932</v>
+      </c>
+      <c r="B36" s="2">
+        <f>SUM(B35+C36)</f>
+        <v>482</v>
+      </c>
+      <c r="C36" s="2">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -832,10 +844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,6 +1242,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>43932</v>
+      </c>
+      <c r="B36" s="2">
+        <f>SUM(B35+C36)</f>
+        <v>36</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1239,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,6 +1666,18 @@
         <v>6</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>43932</v>
+      </c>
+      <c r="B36" s="2">
+        <f>SUM(B35+C36)</f>
+        <v>30</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data update 12 April 20
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Death!$A$1:$C$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Recoverd!$A$1:$C$28</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B36"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f>SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B37" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -776,7 +776,7 @@
         <v>43928</v>
       </c>
       <c r="B32" s="2">
-        <f>SUM(B31+C32)</f>
+        <f t="shared" si="0"/>
         <v>164</v>
       </c>
       <c r="C32" s="2">
@@ -788,7 +788,7 @@
         <v>43929</v>
       </c>
       <c r="B33" s="2">
-        <f>SUM(B32+C33)</f>
+        <f t="shared" si="0"/>
         <v>218</v>
       </c>
       <c r="C33" s="2">
@@ -800,7 +800,7 @@
         <v>43930</v>
       </c>
       <c r="B34" s="2">
-        <f>SUM(B33+C34)</f>
+        <f t="shared" si="0"/>
         <v>330</v>
       </c>
       <c r="C34" s="2">
@@ -812,7 +812,7 @@
         <v>43931</v>
       </c>
       <c r="B35" s="2">
-        <f>SUM(B34+C35)</f>
+        <f t="shared" si="0"/>
         <v>424</v>
       </c>
       <c r="C35" s="2">
@@ -824,11 +824,23 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f>SUM(B35+C36)</f>
+        <f t="shared" si="0"/>
         <v>482</v>
       </c>
       <c r="C36" s="2">
         <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>43933</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="0"/>
+        <v>621</v>
+      </c>
+      <c r="C37" s="2">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -844,10 +856,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,6 +1266,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>43933</v>
+      </c>
+      <c r="B37" s="2">
+        <f>SUM(B36+C37)</f>
+        <v>36</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1263,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1635,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f>SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B37" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -1623,7 +1647,7 @@
         <v>43928</v>
       </c>
       <c r="B32" s="2">
-        <f>SUM(B31+C32)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C32" s="2">
@@ -1635,7 +1659,7 @@
         <v>43929</v>
       </c>
       <c r="B33" s="2">
-        <f>SUM(B32+C33)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C33" s="2">
@@ -1647,7 +1671,7 @@
         <v>43930</v>
       </c>
       <c r="B34" s="2">
-        <f>SUM(B33+C34)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C34" s="2">
@@ -1659,7 +1683,7 @@
         <v>43931</v>
       </c>
       <c r="B35" s="2">
-        <f>SUM(B34+C35)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C35" s="2">
@@ -1671,11 +1695,23 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f>SUM(B35+C36)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C36" s="2">
         <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>43933</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data and power bi update to 12 april 20
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -858,7 +858,438 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>43898</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>43899</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>43900</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>43901</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>43902</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>43903</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>43904</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>43905</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>43906</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>43907</v>
+      </c>
+      <c r="B11" s="2">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>43908</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>43909</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>43910</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>43911</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>43912</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>43913</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>43914</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>43915</v>
+      </c>
+      <c r="B19" s="2">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>43916</v>
+      </c>
+      <c r="B20" s="2">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>43917</v>
+      </c>
+      <c r="B21" s="2">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>43918</v>
+      </c>
+      <c r="B22" s="2">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>43919</v>
+      </c>
+      <c r="B23" s="2">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>43920</v>
+      </c>
+      <c r="B24" s="2">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>43921</v>
+      </c>
+      <c r="B25" s="2">
+        <v>25</v>
+      </c>
+      <c r="C25" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>43922</v>
+      </c>
+      <c r="B26" s="2">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>43923</v>
+      </c>
+      <c r="B27" s="2">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>43924</v>
+      </c>
+      <c r="B28" s="2">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>43925</v>
+      </c>
+      <c r="B29" s="2">
+        <v>30</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>43926</v>
+      </c>
+      <c r="B30" s="2">
+        <v>33</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>43927</v>
+      </c>
+      <c r="B31" s="2">
+        <v>33</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>43928</v>
+      </c>
+      <c r="B32" s="2">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>43929</v>
+      </c>
+      <c r="B33" s="2">
+        <v>33</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>43930</v>
+      </c>
+      <c r="B34" s="2">
+        <v>33</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>43931</v>
+      </c>
+      <c r="B35" s="2">
+        <v>33</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>43932</v>
+      </c>
+      <c r="B36" s="2">
+        <f>SUM(B35+C36)</f>
+        <v>36</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>43933</v>
+      </c>
+      <c r="B37" s="2">
+        <f>SUM(B36+C37)</f>
+        <v>39</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C28"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -874,437 +1305,6 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>43898</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>43899</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>43900</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>43901</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>43902</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>43903</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>43904</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>43905</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>43906</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>43907</v>
-      </c>
-      <c r="B11" s="2">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>43908</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>43909</v>
-      </c>
-      <c r="B13" s="2">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>43910</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>43911</v>
-      </c>
-      <c r="B15" s="2">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>43912</v>
-      </c>
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>43913</v>
-      </c>
-      <c r="B17" s="2">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>43914</v>
-      </c>
-      <c r="B18" s="2">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>43915</v>
-      </c>
-      <c r="B19" s="2">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>43916</v>
-      </c>
-      <c r="B20" s="2">
-        <v>11</v>
-      </c>
-      <c r="C20" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>43917</v>
-      </c>
-      <c r="B21" s="2">
-        <v>11</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>43918</v>
-      </c>
-      <c r="B22" s="2">
-        <v>15</v>
-      </c>
-      <c r="C22" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>43919</v>
-      </c>
-      <c r="B23" s="2">
-        <v>15</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>43920</v>
-      </c>
-      <c r="B24" s="2">
-        <v>19</v>
-      </c>
-      <c r="C24" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>43921</v>
-      </c>
-      <c r="B25" s="2">
-        <v>25</v>
-      </c>
-      <c r="C25" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>43922</v>
-      </c>
-      <c r="B26" s="2">
-        <v>25</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>43923</v>
-      </c>
-      <c r="B27" s="2">
-        <v>25</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>43924</v>
-      </c>
-      <c r="B28" s="2">
-        <v>26</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>43925</v>
-      </c>
-      <c r="B29" s="2">
-        <v>30</v>
-      </c>
-      <c r="C29" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>43926</v>
-      </c>
-      <c r="B30" s="2">
-        <v>33</v>
-      </c>
-      <c r="C30" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>43927</v>
-      </c>
-      <c r="B31" s="2">
-        <v>33</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>43928</v>
-      </c>
-      <c r="B32" s="2">
-        <v>33</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>43929</v>
-      </c>
-      <c r="B33" s="2">
-        <v>33</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>43930</v>
-      </c>
-      <c r="B34" s="2">
-        <v>33</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>43931</v>
-      </c>
-      <c r="B35" s="2">
-        <v>33</v>
-      </c>
-      <c r="C35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>43932</v>
-      </c>
-      <c r="B36" s="2">
-        <f>SUM(B35+C36)</f>
-        <v>36</v>
-      </c>
-      <c r="C36" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>43933</v>
-      </c>
-      <c r="B37" s="2">
-        <f>SUM(B36+C37)</f>
-        <v>36</v>
-      </c>
-      <c r="C37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C28"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="3" t="s">

</xml_diff>

<commit_message>
update 13 april dataset
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B37" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B38" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -841,6 +841,18 @@
       </c>
       <c r="C37" s="2">
         <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>43934</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" si="0"/>
+        <v>803</v>
+      </c>
+      <c r="C38" s="2">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -856,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,6 +1290,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>43934</v>
+      </c>
+      <c r="B38" s="2">
+        <f>SUM(B37+C38)</f>
+        <v>42</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1287,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,7 +1659,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B37" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B38" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -1712,6 +1736,18 @@
       </c>
       <c r="C37" s="2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>43934</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C38" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dataset update 15 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B39" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B40" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -865,6 +865,18 @@
       </c>
       <c r="C39" s="2">
         <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>43936</v>
+      </c>
+      <c r="B40" s="2">
+        <f t="shared" si="0"/>
+        <v>1231</v>
+      </c>
+      <c r="C40" s="2">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -880,7 +892,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
@@ -1326,6 +1338,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>43936</v>
+      </c>
+      <c r="B40" s="2">
+        <f>SUM(B39+C40)</f>
+        <v>49</v>
+      </c>
+      <c r="C40" s="2">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1335,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1707,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B39" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B40" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -1784,6 +1808,18 @@
       </c>
       <c r="C39" s="2">
         <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>43936</v>
+      </c>
+      <c r="B40" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update dataset to 16 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B40" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B41" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -877,6 +877,18 @@
       </c>
       <c r="C40" s="2">
         <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>43937</v>
+      </c>
+      <c r="B41" s="2">
+        <f t="shared" si="0"/>
+        <v>1572</v>
+      </c>
+      <c r="C41" s="2">
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -892,10 +904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,6 +1362,18 @@
         <v>7</v>
       </c>
     </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>43937</v>
+      </c>
+      <c r="B41" s="2">
+        <f>SUM(B40+C41)</f>
+        <v>49</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C28"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1359,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1731,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B40" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B41" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -1820,6 +1844,18 @@
       </c>
       <c r="C40" s="2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>43937</v>
+      </c>
+      <c r="B41" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C41" s="2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dataset update 17 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B41" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B42" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -889,6 +889,18 @@
       </c>
       <c r="C41" s="2">
         <v>341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>43938</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" si="0"/>
+        <v>1838</v>
+      </c>
+      <c r="C42" s="2">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -904,10 +916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:B41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1319,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f>SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B42" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -1319,7 +1331,7 @@
         <v>43933</v>
       </c>
       <c r="B37" s="2">
-        <f>SUM(B36+C37)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="C37" s="2">
@@ -1331,7 +1343,7 @@
         <v>43934</v>
       </c>
       <c r="B38" s="2">
-        <f>SUM(B37+C38)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="C38" s="2">
@@ -1343,7 +1355,7 @@
         <v>43935</v>
       </c>
       <c r="B39" s="2">
-        <f>SUM(B38+C39)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="C39" s="2">
@@ -1355,7 +1367,7 @@
         <v>43936</v>
       </c>
       <c r="B40" s="2">
-        <f>SUM(B39+C40)</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="C40" s="2">
@@ -1367,11 +1379,23 @@
         <v>43937</v>
       </c>
       <c r="B41" s="2">
-        <f>SUM(B40+C41)</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="C41" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>43938</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="C42" s="2">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1383,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:B41"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1755,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B41" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B42" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -1856,6 +1880,18 @@
       </c>
       <c r="C41" s="2">
         <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>43938</v>
+      </c>
+      <c r="B42" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C42" s="2">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dataset update and power bi file update
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:B43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B43" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B44" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -913,6 +913,18 @@
       </c>
       <c r="C43" s="2">
         <v>306</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43940</v>
+      </c>
+      <c r="B44" s="2">
+        <f t="shared" si="0"/>
+        <v>2456</v>
+      </c>
+      <c r="C44" s="2">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -928,10 +940,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:B43"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1343,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:B43" si="0">SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B44" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -1420,6 +1432,18 @@
       </c>
       <c r="C43" s="2">
         <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43940</v>
+      </c>
+      <c r="B44" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C44" s="2">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1431,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:B43"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +1803,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B43" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B44" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -1928,6 +1952,18 @@
       </c>
       <c r="C43" s="2">
         <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43940</v>
+      </c>
+      <c r="B44" s="2">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="C44" s="2">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
power bi file update and new report published
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:B51"/>
+      <selection activeCell="B50" sqref="B50:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:B51"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update upto 27 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B51" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B52" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -1009,6 +1009,18 @@
       </c>
       <c r="C51" s="2">
         <v>418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>43948</v>
+      </c>
+      <c r="B52" s="2">
+        <f t="shared" si="0"/>
+        <v>5913</v>
+      </c>
+      <c r="C52" s="2">
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -1024,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:B51"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1439,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:B51" si="0">SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B52" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -1611,6 +1623,18 @@
         <v>122</v>
       </c>
       <c r="C51" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>43948</v>
+      </c>
+      <c r="B52" s="2">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="C52" s="2">
         <v>9</v>
       </c>
     </row>
@@ -1623,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:B51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1971,7 +1995,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B51" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B52" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -2216,6 +2240,18 @@
       </c>
       <c r="C51" s="2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>43948</v>
+      </c>
+      <c r="B52" s="2">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="C52" s="2">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file update to 28 april
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B52" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B53" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -1021,6 +1021,18 @@
       </c>
       <c r="C52" s="2">
         <v>497</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>43949</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" si="0"/>
+        <v>6462</v>
+      </c>
+      <c r="C53" s="2">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -1036,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1451,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:B52" si="0">SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B53" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -1636,6 +1648,18 @@
       </c>
       <c r="C52" s="2">
         <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>43949</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="C53" s="2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1647,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,7 +2019,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B52" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B53" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -2252,6 +2276,18 @@
       </c>
       <c r="C52" s="2">
         <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>43949</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data update to 23 may
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -1350,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77:B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,7 +1751,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:B77" si="0">SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B78" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -2253,6 +2253,13 @@
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>43974</v>
+      </c>
+      <c r="B78" s="2">
+        <f t="shared" si="0"/>
+        <v>6486</v>
+      </c>
+      <c r="C78" s="2">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2266,7 +2273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data update 30 may
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:B84"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84:B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B84" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B85" si="0">SUM(B30+C31)</f>
         <v>123</v>
       </c>
       <c r="C31" s="2">
@@ -1405,6 +1405,18 @@
       </c>
       <c r="C84" s="2">
         <v>2523</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>43981</v>
+      </c>
+      <c r="B85" s="2">
+        <f t="shared" si="0"/>
+        <v>44608</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1764</v>
       </c>
     </row>
   </sheetData>
@@ -1420,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:B84"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84:B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,7 +1835,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:B84" si="0">SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B85" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -2404,6 +2416,18 @@
       </c>
       <c r="C84" s="2">
         <v>590</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>43981</v>
+      </c>
+      <c r="B85" s="2">
+        <f t="shared" si="0"/>
+        <v>9375</v>
+      </c>
+      <c r="C85" s="2">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -2415,10 +2439,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:B84"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84:B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,7 +2787,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B84" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B85" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -3404,6 +3428,18 @@
       </c>
       <c r="C84" s="2">
         <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>43981</v>
+      </c>
+      <c r="B85" s="2">
+        <f t="shared" si="0"/>
+        <v>610</v>
+      </c>
+      <c r="C85" s="2">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data update 11 june 20
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:B96"/>
+      <selection activeCell="B96" sqref="B96:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,6 +1549,18 @@
       </c>
       <c r="C96" s="2">
         <v>3190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>43993</v>
+      </c>
+      <c r="B97" s="2">
+        <f>SUM(B96+C97)</f>
+        <v>78052</v>
+      </c>
+      <c r="C97" s="2">
+        <v>3187</v>
       </c>
     </row>
   </sheetData>
@@ -1564,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:B96"/>
+      <selection activeCell="B96" sqref="B96:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1979,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:B96" si="0">SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B97" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -2692,6 +2704,18 @@
       </c>
       <c r="C96" s="2">
         <v>563</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>43993</v>
+      </c>
+      <c r="B97" s="2">
+        <f t="shared" si="0"/>
+        <v>16748</v>
+      </c>
+      <c r="C97" s="2">
+        <v>848</v>
       </c>
     </row>
   </sheetData>
@@ -2703,10 +2727,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:B96"/>
+      <selection activeCell="B96" sqref="B96:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,7 +3075,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B96" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B97" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -3835,6 +3859,18 @@
         <v>1012</v>
       </c>
       <c r="C96" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>43993</v>
+      </c>
+      <c r="B97" s="2">
+        <f t="shared" si="0"/>
+        <v>1049</v>
+      </c>
+      <c r="C97" s="2">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data update 12 june 20
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96:B97"/>
+      <selection activeCell="B97" sqref="B97:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1496,7 @@
         <v>43988</v>
       </c>
       <c r="B92" s="2">
-        <f>SUM(B91+C92)</f>
+        <f t="shared" ref="B92:B98" si="1">SUM(B91+C92)</f>
         <v>63026</v>
       </c>
       <c r="C92" s="2">
@@ -1508,7 +1508,7 @@
         <v>43989</v>
       </c>
       <c r="B93" s="2">
-        <f>SUM(B92+C93)</f>
+        <f t="shared" si="1"/>
         <v>65769</v>
       </c>
       <c r="C93" s="2">
@@ -1520,7 +1520,7 @@
         <v>43990</v>
       </c>
       <c r="B94" s="2">
-        <f>SUM(B93+C94)</f>
+        <f t="shared" si="1"/>
         <v>68504</v>
       </c>
       <c r="C94" s="2">
@@ -1532,7 +1532,7 @@
         <v>43991</v>
       </c>
       <c r="B95" s="2">
-        <f>SUM(B94+C95)</f>
+        <f t="shared" si="1"/>
         <v>71675</v>
       </c>
       <c r="C95" s="2">
@@ -1544,7 +1544,7 @@
         <v>43992</v>
       </c>
       <c r="B96" s="2">
-        <f>SUM(B95+C96)</f>
+        <f t="shared" si="1"/>
         <v>74865</v>
       </c>
       <c r="C96" s="2">
@@ -1556,11 +1556,23 @@
         <v>43993</v>
       </c>
       <c r="B97" s="2">
-        <f>SUM(B96+C97)</f>
+        <f t="shared" si="1"/>
         <v>78052</v>
       </c>
       <c r="C97" s="2">
         <v>3187</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>43994</v>
+      </c>
+      <c r="B98" s="2">
+        <f t="shared" si="1"/>
+        <v>81523</v>
+      </c>
+      <c r="C98" s="2">
+        <v>3471</v>
       </c>
     </row>
   </sheetData>
@@ -1576,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96:B97"/>
+      <selection activeCell="B97" sqref="B97:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +1991,7 @@
         <v>43932</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" ref="B36:B97" si="0">SUM(B35+C36)</f>
+        <f t="shared" ref="B36:B98" si="0">SUM(B35+C36)</f>
         <v>36</v>
       </c>
       <c r="C36" s="2">
@@ -2716,6 +2728,18 @@
       </c>
       <c r="C97" s="2">
         <v>848</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>43994</v>
+      </c>
+      <c r="B98" s="2">
+        <f t="shared" si="0"/>
+        <v>17250</v>
+      </c>
+      <c r="C98" s="2">
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -2727,10 +2751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96:B97"/>
+      <selection activeCell="B97" sqref="B97:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3075,7 +3099,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B97" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B98" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -3872,6 +3896,18 @@
       </c>
       <c r="C97" s="2">
         <v>37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>43994</v>
+      </c>
+      <c r="B98" s="2">
+        <f t="shared" si="0"/>
+        <v>1095</v>
+      </c>
+      <c r="C98" s="2">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data update 2 july
</commit_message>
<xml_diff>
--- a/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
+++ b/DataSheet/COVID-19_Bangladesh_DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Confirmed" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116:B117"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1496,7 @@
         <v>43988</v>
       </c>
       <c r="B92" s="2">
-        <f t="shared" ref="B92:B117" si="1">SUM(B91+C92)</f>
+        <f t="shared" ref="B92:B118" si="1">SUM(B91+C92)</f>
         <v>63026</v>
       </c>
       <c r="C92" s="2">
@@ -1801,6 +1801,18 @@
       </c>
       <c r="C117" s="2">
         <v>3775</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>44014</v>
+      </c>
+      <c r="B118" s="2">
+        <f t="shared" si="1"/>
+        <v>153277</v>
+      </c>
+      <c r="C118" s="2">
+        <v>4019</v>
       </c>
     </row>
   </sheetData>
@@ -1816,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116:B117"/>
+      <selection activeCell="B117" sqref="B117:B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,7 +3023,7 @@
         <v>43998</v>
       </c>
       <c r="B102" s="2">
-        <f t="shared" ref="B102:B117" si="1">SUM(B101+C102)</f>
+        <f t="shared" ref="B102:B118" si="1">SUM(B101+C102)</f>
         <v>36264</v>
       </c>
       <c r="C102" s="2">
@@ -3196,6 +3208,18 @@
       </c>
       <c r="C117" s="2">
         <v>2884</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>44014</v>
+      </c>
+      <c r="B118" s="2">
+        <f t="shared" si="1"/>
+        <v>66842</v>
+      </c>
+      <c r="C118" s="2">
+        <v>4334</v>
       </c>
     </row>
   </sheetData>
@@ -3207,10 +3231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116:B117"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3555,7 +3579,7 @@
         <v>43927</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" ref="B31:B117" si="0">SUM(B30+C31)</f>
+        <f t="shared" ref="B31:B118" si="0">SUM(B30+C31)</f>
         <v>12</v>
       </c>
       <c r="C31" s="2">
@@ -4592,6 +4616,18 @@
       </c>
       <c r="C117" s="2">
         <v>41</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>44014</v>
+      </c>
+      <c r="B118" s="2">
+        <f t="shared" si="0"/>
+        <v>1926</v>
+      </c>
+      <c r="C118" s="2">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>